<commit_message>
added spec for fix
</commit_message>
<xml_diff>
--- a/spec/files/penetrations.xlsx
+++ b/spec/files/penetrations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="118">
   <si>
     <t xml:space="preserve">PLZ</t>
   </si>
@@ -326,7 +326,16 @@
     <t xml:space="preserve">Denens</t>
   </si>
   <si>
-    <t xml:space="preserve">Bussy-Chardonney</t>
+    <t xml:space="preserve">Bussy-Chardonney </t>
+  </si>
+  <si>
+    <t xml:space="preserve">G.fast </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticino </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Land </t>
   </si>
   <si>
     <t xml:space="preserve">Sévery</t>
@@ -345,6 +354,12 @@
   </si>
   <si>
     <t xml:space="preserve">Mollens (VD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mollens (VD) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ost Agglomeration Winterthur </t>
   </si>
   <si>
     <t xml:space="preserve">KAM Region</t>
@@ -466,7 +481,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -485,6 +500,10 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -579,12 +598,12 @@
   <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D107" activeCellId="0" sqref="D107"/>
+      <selection pane="bottomLeft" activeCell="H94" activeCellId="0" sqref="H94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.75"/>
@@ -2745,16 +2764,16 @@
         <v>0.410112359550562</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2762,7 +2781,7 @@
         <v>1141</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C95" s="4" t="n">
         <v>0.232758620689655</v>
@@ -2785,7 +2804,7 @@
         <v>1142</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C96" s="4" t="n">
         <v>0.18</v>
@@ -2831,7 +2850,7 @@
         <v>1144</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C98" s="4" t="n">
         <v>0</v>
@@ -2854,7 +2873,7 @@
         <v>1145</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C99" s="4" t="n">
         <v>0.63</v>
@@ -2877,13 +2896,13 @@
         <v>1147</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C100" s="4" t="n">
         <v>0</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>16</v>
@@ -2900,13 +2919,13 @@
         <v>1147</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C101" s="4" t="n">
         <v>0</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>24</v>
@@ -2923,7 +2942,7 @@
         <v>1148</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C102" s="4" t="n">
         <v>2</v>
@@ -2938,6 +2957,29 @@
         <v>19</v>
       </c>
       <c r="G102" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="n">
+        <v>1149</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C103" s="5" t="n">
+        <v>0.1012</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F103" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G103" s="0" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2969,7 +3011,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.38"/>
@@ -2982,37 +3024,37 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>108</v>
+      <c r="G1" s="6" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -3067,14 +3109,14 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>